<commit_message>
update generated DQ reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">PatientIdentifikator</t>
   </si>
@@ -156,15 +156,6 @@
     <t xml:space="preserve">case_no_py</t>
   </si>
   <si>
-    <t xml:space="preserve">rdCase_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orphaCase_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tracerCase_no_py</t>
-  </si>
-  <si>
     <t xml:space="preserve">rdCase_rel_py_ipat</t>
   </si>
   <si>
@@ -175,24 +166,6 @@
   </si>
   <si>
     <t xml:space="preserve">missing_item_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing_value_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orphaMissing_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implausible_codeLink_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">outlier_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ambiguous_rdCase_no_py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duplicateRdCase_no_py</t>
   </si>
   <si>
     <t xml:space="preserve">dataFormat</t>
@@ -793,37 +766,10 @@
       <c r="S1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
         <v>2020</v>
@@ -856,53 +802,26 @@
         <v>45</v>
       </c>
       <c r="L2" t="n">
-        <v>27</v>
+        <v>2708</v>
       </c>
       <c r="M2" t="n">
-        <v>23</v>
+        <v>2307</v>
       </c>
       <c r="N2" t="n">
-        <v>11</v>
+        <v>1103</v>
       </c>
       <c r="O2" t="n">
-        <v>2708</v>
-      </c>
-      <c r="P2" t="n">
-        <v>2307</v>
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
       </c>
       <c r="Q2" t="n">
-        <v>1103</v>
-      </c>
-      <c r="R2" t="n">
-        <v>3</v>
-      </c>
-      <c r="S2" t="n">
-        <v>5</v>
-      </c>
-      <c r="T2" t="n">
-        <v>5</v>
-      </c>
-      <c r="U2" t="n">
-        <v>3</v>
-      </c>
-      <c r="V2" t="n">
-        <v>1</v>
-      </c>
-      <c r="W2" t="n">
-        <v>3</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="AA2"/>
-      <c r="AB2" t="s">
-        <v>66</v>
+        <v>0.05</v>
+      </c>
+      <c r="R2"/>
+      <c r="S2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update required DQ reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
@@ -13,21 +13,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
-  <si>
-    <t xml:space="preserve">PatientIdentifikator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmenummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICD_Primaerkode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orpha_Kode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dq_msg</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+  <si>
+    <t xml:space="preserve">Patient ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admission ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICD_Primary Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orphacode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DQ_Violations</t>
   </si>
   <si>
     <t xml:space="preserve">260123451-Airolo-P-0000251</t>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">797</t>
   </si>
   <si>
-    <t xml:space="preserve">Implausible birthdate 1877-12-01 maximal age 105. </t>
+    <t xml:space="preserve">Implausible birthdate 1877-12-01 maximal age 130. </t>
   </si>
   <si>
     <t xml:space="preserve">260123451-Airolo-P-0000100</t>
@@ -156,6 +156,39 @@
     <t xml:space="preserve">case_no_py</t>
   </si>
   <si>
+    <t xml:space="preserve">missing_item_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing_value_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outlier_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orphaMissing_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implausible_codeLink_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambiguous_rdCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duplicateRdCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mxCases_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orphaCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tracerCase_no_py</t>
+  </si>
+  <si>
     <t xml:space="preserve">rdCase_rel_py_ipat</t>
   </si>
   <si>
@@ -165,28 +198,31 @@
     <t xml:space="preserve">tracerCase_rel_py_ipat</t>
   </si>
   <si>
-    <t xml:space="preserve">missing_item_no_py</t>
+    <t xml:space="preserve">executionTime_inMin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateRef</t>
   </si>
   <si>
     <t xml:space="preserve">dataFormat</t>
   </si>
   <si>
-    <t xml:space="preserve">executionTime_inMin</t>
+    <t xml:space="preserve">diagnosesList</t>
   </si>
   <si>
     <t xml:space="preserve">encounterClass</t>
   </si>
   <si>
-    <t xml:space="preserve">dateRef</t>
-  </si>
-  <si>
     <t xml:space="preserve">260123451-Airolo</t>
   </si>
   <si>
+    <t xml:space="preserve">Diagnosedatum</t>
+  </si>
+  <si>
     <t xml:space="preserve">FHIR</t>
   </si>
   <si>
-    <t xml:space="preserve">Diagnosedatum</t>
+    <t xml:space="preserve">v1</t>
   </si>
 </sst>
 </file>
@@ -194,13 +230,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,8 +265,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,21 +560,28 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="26.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="26.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="16.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="9.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="101.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -683,16 +733,9 @@
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
-      <c r="E11"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -707,69 +750,134 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="22.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="29.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="29.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="23.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="25.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="15.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="10.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="18.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="19.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="13.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="18.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="26.71" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="22.71" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="21.71" hidden="0" customWidth="1"/>
+    <col min="19" max="19" width="12.71" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="13.71" hidden="0" customWidth="1"/>
+    <col min="21" max="21" width="15.71" hidden="0" customWidth="1"/>
+    <col min="22" max="22" width="16.71" hidden="0" customWidth="1"/>
+    <col min="23" max="23" width="18.71" hidden="0" customWidth="1"/>
+    <col min="24" max="24" width="21.71" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="22.71" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="19.71" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="13.71" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="10.71" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="13.71" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="14.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B2" t="n">
         <v>2020</v>
@@ -802,27 +910,60 @@
         <v>45</v>
       </c>
       <c r="L2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>5</v>
+      </c>
+      <c r="P2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>27</v>
+      </c>
+      <c r="T2" t="n">
+        <v>18</v>
+      </c>
+      <c r="U2" t="n">
+        <v>23</v>
+      </c>
+      <c r="V2" t="n">
+        <v>11</v>
+      </c>
+      <c r="W2" t="n">
         <v>2708</v>
       </c>
-      <c r="M2" t="n">
+      <c r="X2" t="n">
         <v>2307</v>
       </c>
-      <c r="N2" t="n">
+      <c r="Y2" t="n">
         <v>1103</v>
       </c>
-      <c r="O2" t="n">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="R2"/>
-      <c r="S2" t="s">
-        <v>57</v>
-      </c>
+      <c r="Z2" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add parallel computing optimization
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t xml:space="preserve">Abbreviation</t>
   </si>
@@ -102,21 +102,21 @@
     <t xml:space="preserve">RD Case Dissimilarity Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">aCase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyzed Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
     <t xml:space="preserve">aPatient</t>
   </si>
   <si>
     <t xml:space="preserve">Analyzed Patients</t>
   </si>
   <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aCase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analyzed Cases</t>
-  </si>
-  <si>
     <t xml:space="preserve">im_misg</t>
   </si>
   <si>
@@ -240,7 +240,16 @@
     <t xml:space="preserve">Execution Time</t>
   </si>
   <si>
-    <t xml:space="preserve">0.08</t>
+    <t xml:space="preserve">0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cpu_core</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU cores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">date_ref</t>
@@ -291,6 +300,27 @@
     <t xml:space="preserve">DQ_Violations</t>
   </si>
   <si>
+    <t xml:space="preserve">260123451-Airolo-P-0000247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260123451-Airolo-F-0000255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E84.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing Orpha Code.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E84.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260123451-Airolo-P-0000248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260123451-Airolo-F-0000256</t>
+  </si>
+  <si>
     <t xml:space="preserve">260123451-Airolo-P-0000251</t>
   </si>
   <si>
@@ -300,7 +330,13 @@
     <t xml:space="preserve">E84.9</t>
   </si>
   <si>
-    <t xml:space="preserve">Missing Orpha Code.  </t>
+    <t xml:space="preserve">260123451-Airolo-P-0000527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260123451-Airolo-F-0000545</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E84.80</t>
   </si>
   <si>
     <t xml:space="preserve">260123451-Airolo-P-0000002</t>
@@ -342,24 +378,6 @@
     <t xml:space="preserve">Ambiguous Orphacoding. ICD10-Orpha combination: E03.1 - 797 is implausible according to Alpha-ID-SE. </t>
   </si>
   <si>
-    <t xml:space="preserve">260123451-Airolo-P-0000247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260123451-Airolo-F-0000255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E84.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E84.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260123451-Airolo-P-0000248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260123451-Airolo-F-0000256</t>
-  </si>
-  <si>
     <t xml:space="preserve">260123451-Airolo-P-0000345</t>
   </si>
   <si>
@@ -370,15 +388,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ambiguous Orphacoding. ICD10-Orpha combination: E03.1 - 442 is implausible according to Alpha-ID-SE. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">260123451-Airolo-P-0000527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260123451-Airolo-F-0000545</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E84.80</t>
   </si>
   <si>
     <t xml:space="preserve">Following items are missing:  Kontakt_Klasse , Fall_Status , DiagnoseRolle</t>
@@ -1062,7 +1071,18 @@
       <c r="B31" t="s">
         <v>86</v>
       </c>
-      <c r="C31"/>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,115 +1107,111 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
       <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="s">
         <v>98</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
       <c r="C4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" t="s">
         <v>99</v>
       </c>
+      <c r="D4"/>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D5"/>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
         <v>109</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>110</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
         <v>112</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8">
@@ -1206,43 +1222,47 @@
         <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8"/>
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
         <v>119</v>
       </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10"/>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
@@ -1251,7 +1271,7 @@
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add automatic detection of CPU cores
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t xml:space="preserve">Abbreviation</t>
   </si>
@@ -24,19 +24,28 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">st_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORD-MI</t>
+  </si>
+  <si>
     <t xml:space="preserve">org_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Organization Name or Identifier </t>
+    <t xml:space="preserve">Organization Name or Identifier</t>
   </si>
   <si>
     <t xml:space="preserve">260123451-Airolo</t>
   </si>
   <si>
-    <t xml:space="preserve">rep_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report Year</t>
+    <t xml:space="preserve">rep_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Date (refers to the date or year of data acquisition)</t>
   </si>
   <si>
     <t xml:space="preserve">2020</t>
@@ -240,7 +249,16 @@
     <t xml:space="preserve">Execution Time</t>
   </si>
   <si>
-    <t xml:space="preserve">0.04</t>
+    <t xml:space="preserve">0.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">par_computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance Optimization for Parallel Computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">cpu_core</t>
@@ -249,7 +267,7 @@
     <t xml:space="preserve">CPU cores</t>
   </si>
   <si>
-    <t xml:space="preserve">4</t>
+    <t xml:space="preserve">8</t>
   </si>
   <si>
     <t xml:space="preserve">date_ref</t>
@@ -261,7 +279,7 @@
     <t xml:space="preserve">Diagnosedatum</t>
   </si>
   <si>
-    <t xml:space="preserve">dataFormat</t>
+    <t xml:space="preserve">data_format</t>
   </si>
   <si>
     <t xml:space="preserve">Data Format</t>
@@ -270,7 +288,7 @@
     <t xml:space="preserve">FHIR</t>
   </si>
   <si>
-    <t xml:space="preserve">dxList</t>
+    <t xml:space="preserve">dx_list</t>
   </si>
   <si>
     <t xml:space="preserve">Version of Used Diagnosis List</t>
@@ -279,7 +297,7 @@
     <t xml:space="preserve">v1</t>
   </si>
   <si>
-    <t xml:space="preserve">enctrClass</t>
+    <t xml:space="preserve">enctr_class</t>
   </si>
   <si>
     <t xml:space="preserve">Encounter Class</t>
@@ -730,7 +748,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="32.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="60.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="16.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -841,18 +859,18 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -863,18 +881,18 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14">
@@ -918,26 +936,26 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -945,13 +963,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21">
@@ -1082,7 +1100,29 @@
       <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="C32"/>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1107,162 +1147,162 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
         <v>117</v>
       </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" t="s">
-        <v>111</v>
-      </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11">
@@ -1271,7 +1311,7 @@
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update documentation and required packages
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_meDIC_StandortName_FHIR_2020.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t xml:space="preserve">Abbreviation</t>
   </si>
@@ -189,15 +189,6 @@
     <t xml:space="preserve">27</t>
   </si>
   <si>
-    <t xml:space="preserve">mxCase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixed Cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
     <t xml:space="preserve">orphaCase</t>
   </si>
   <si>
@@ -249,7 +240,7 @@
     <t xml:space="preserve">Execution Time</t>
   </si>
   <si>
-    <t xml:space="preserve">0.08</t>
+    <t xml:space="preserve">0.06</t>
   </si>
   <si>
     <t xml:space="preserve">par_computing</t>
@@ -1111,18 +1102,7 @@
       <c r="B33" t="s">
         <v>92</v>
       </c>
-      <c r="C33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34"/>
+      <c r="C33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1147,162 +1127,162 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
         <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>105</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
         <v>114</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" t="s">
         <v>119</v>
-      </c>
-      <c r="B8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" t="s">
         <v>123</v>
-      </c>
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" t="s">
         <v>127</v>
-      </c>
-      <c r="B10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="11">
@@ -1311,7 +1291,7 @@
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>